<commit_message>
polish the syllabi mapping data. update the rendered course codes and add mapping
</commit_message>
<xml_diff>
--- a/data/processed_scores.xlsx
+++ b/data/processed_scores.xlsx
@@ -554,731 +554,731 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>APSC 383</t>
+          <t>BAEN 580</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.225077636539936</v>
+        <v>0.6776421144604683</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6893610060214996</v>
+        <v>0.7572773620486259</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5513069182634354</v>
+        <v>0.8760410100221634</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4186507612466812</v>
+        <v>0.5903653390705585</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3057575821876526</v>
+        <v>0.5230860859155655</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4233366549015045</v>
+        <v>0.6300440952181816</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1879539787769317</v>
+        <v>0.8363740146160126</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0409446209669113</v>
+        <v>0.0790983934421092</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1995269060134887</v>
+        <v>0.2010860694572329</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1937873214483261</v>
+        <v>0.4891903721727431</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2508588880300522</v>
+        <v>0.1931973490864038</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1923822909593582</v>
+        <v>0.2247700709849596</v>
       </c>
       <c r="N2" t="n">
-        <v>0.4476391971111297</v>
+        <v>0.2753241355530917</v>
       </c>
       <c r="O2" t="n">
-        <v>0.5635110065340996</v>
+        <v>0.5269269123673439</v>
       </c>
       <c r="P2" t="n">
-        <v>0.2413162365555763</v>
+        <v>0.4770326390862465</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2752360552549362</v>
+        <v>0.5960461348295212</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2399156466126442</v>
+        <v>0.7274299878627062</v>
       </c>
       <c r="S2" t="n">
-        <v>0.519437164068222</v>
+        <v>0.5293902922421694</v>
       </c>
       <c r="T2" t="n">
-        <v>0.6512212306261063</v>
+        <v>0.8018344193696976</v>
       </c>
       <c r="U2" t="n">
-        <v>0.0901582948863506</v>
+        <v>0.3202038947492838</v>
       </c>
       <c r="V2" t="n">
-        <v>0.4331253916025162</v>
+        <v>0.3311157487332821</v>
       </c>
       <c r="W2" t="n">
-        <v>0.5061413943767548</v>
+        <v>0.5707065239548683</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>APSC 440</t>
+          <t>BAPA 580</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2606846988201141</v>
+        <v>0.2472854813871284</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7093207836151123</v>
+        <v>0.5908645888169607</v>
       </c>
       <c r="D3" t="n">
-        <v>0.513254702091217</v>
+        <v>0.3554305862635374</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8721046447753906</v>
+        <v>0.7287373741467794</v>
       </c>
       <c r="F3" t="n">
-        <v>0.185085117816925</v>
+        <v>0.4082688962419827</v>
       </c>
       <c r="G3" t="n">
-        <v>0.1172086000442504</v>
+        <v>0.336679524431626</v>
       </c>
       <c r="H3" t="n">
-        <v>0.0061039207503199</v>
+        <v>0.2482175483213116</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0110382521525025</v>
+        <v>0.2869471477752086</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2069031447172165</v>
+        <v>0.3738296379645665</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2184742987155914</v>
+        <v>0.1793426983058452</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5404530763626099</v>
+        <v>0.2200251342728734</v>
       </c>
       <c r="M3" t="n">
-        <v>0.009191735647618699</v>
+        <v>0.2474037750313679</v>
       </c>
       <c r="N3" t="n">
-        <v>0.0219591930508613</v>
+        <v>0.34411396458745</v>
       </c>
       <c r="O3" t="n">
-        <v>0.8702558279037476</v>
+        <v>0.9326488773028055</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2419787943363189</v>
+        <v>0.1504766469200452</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9971480369567872</v>
+        <v>0.336603802939256</v>
       </c>
       <c r="R3" t="n">
-        <v>0.4427424073219299</v>
+        <v>0.5664254128932953</v>
       </c>
       <c r="S3" t="n">
-        <v>0.5450483560562134</v>
+        <v>0.2654259722524633</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5599349141120911</v>
+        <v>0.7818077603975931</v>
       </c>
       <c r="U3" t="n">
-        <v>0.0108648547902703</v>
+        <v>0.3444054424762726</v>
       </c>
       <c r="V3" t="n">
-        <v>0.5322953462600708</v>
+        <v>0.3947237834023933</v>
       </c>
       <c r="W3" t="n">
-        <v>0.0091787232086062</v>
+        <v>0.0798484074572722</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>APSC 486</t>
+          <t>BAEN 580C</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5838671823342642</v>
+        <v>0.3066916198780139</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6792886257171631</v>
+        <v>0.4349003136157989</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8493436773618063</v>
+        <v>0.2269035100471228</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7451715668042501</v>
+        <v>0.6027461290359497</v>
       </c>
       <c r="F4" t="n">
-        <v>0.6367562015851339</v>
+        <v>0.3717706923683484</v>
       </c>
       <c r="G4" t="n">
-        <v>0.6575605273246765</v>
+        <v>0.2879822670171658</v>
       </c>
       <c r="H4" t="n">
-        <v>0.2406417901317278</v>
+        <v>0.2177003299196561</v>
       </c>
       <c r="I4" t="n">
-        <v>0.22211558263128</v>
+        <v>0.1489402622682973</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2788851782679558</v>
+        <v>0.2691165028760831</v>
       </c>
       <c r="K4" t="n">
-        <v>0.6426869245866934</v>
+        <v>0.2725043430303533</v>
       </c>
       <c r="L4" t="n">
-        <v>0.3509064962466557</v>
+        <v>0.2392489995885019</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3151973485946655</v>
+        <v>0.1319268185955782</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1935244301954905</v>
+        <v>0.09566769733404119</v>
       </c>
       <c r="O4" t="n">
-        <v>0.7736939887205759</v>
+        <v>0.7304885039726893</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3861157620946566</v>
+        <v>0.3128764902551968</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.6769705067078272</v>
+        <v>0.3300680094398558</v>
       </c>
       <c r="R4" t="n">
-        <v>0.5620279088616371</v>
+        <v>0.3150735727200905</v>
       </c>
       <c r="S4" t="n">
-        <v>0.6696630716323853</v>
+        <v>0.3175627046342318</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8885779976844788</v>
+        <v>0.7339196503162384</v>
       </c>
       <c r="U4" t="n">
-        <v>0.2902844001849492</v>
+        <v>0.1526406543950239</v>
       </c>
       <c r="V4" t="n">
-        <v>0.6525993446509043</v>
+        <v>0.2132301593665033</v>
       </c>
       <c r="W4" t="n">
-        <v>0.5568657151112953</v>
+        <v>0.3270305482049783</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>APSC 540</t>
+          <t>BAEN 580A</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7273798495531082</v>
+        <v>0.1834433984414707</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8012893199920654</v>
+        <v>0.413688773555415</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8363658785820007</v>
+        <v>0.3203491995643292</v>
       </c>
       <c r="E5" t="n">
-        <v>0.5632544577121734</v>
+        <v>0.4364164589372064</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5751682817935944</v>
+        <v>0.4117435976596815</v>
       </c>
       <c r="G5" t="n">
-        <v>0.6287448763847351</v>
+        <v>0.2700528663450053</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4008272051811218</v>
+        <v>0.1410570103367458</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1901652626693248</v>
+        <v>0.0620011963016752</v>
       </c>
       <c r="J5" t="n">
-        <v>0.247939270734787</v>
+        <v>0.07591740660635481</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5102368395775556</v>
+        <v>0.1412378432495253</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4511112749576568</v>
+        <v>0.08231207817776259</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2955708980560302</v>
+        <v>0.2699161336557673</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2553298756480217</v>
+        <v>0.2268037516623735</v>
       </c>
       <c r="O5" t="n">
-        <v>0.572181236743927</v>
+        <v>0.7226580168519702</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4163009196519852</v>
+        <v>0.2239315990092499</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.387138120830059</v>
+        <v>0.1580032723556672</v>
       </c>
       <c r="R5" t="n">
-        <v>0.3014095067977905</v>
+        <v>0.4716894509370571</v>
       </c>
       <c r="S5" t="n">
-        <v>0.403736200928688</v>
+        <v>0.0873092199118608</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8502827048301697</v>
+        <v>0.8163535509790693</v>
       </c>
       <c r="U5" t="n">
-        <v>0.4907763734459877</v>
+        <v>0.2775257676839828</v>
       </c>
       <c r="V5" t="n">
-        <v>0.4016070961952209</v>
+        <v>0.1430687305733694</v>
       </c>
       <c r="W5" t="n">
-        <v>0.5666853606700897</v>
+        <v>0.314656164497137</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>BA 560</t>
+          <t>BA 562</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1316252891207114</v>
+        <v>0.2304891447226206</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5403780229389668</v>
+        <v>0.7699000636736552</v>
       </c>
       <c r="D6" t="n">
-        <v>0.377598946611397</v>
+        <v>0.8985457420349121</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4272289484739303</v>
+        <v>0.4081504742304484</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3086892465595156</v>
+        <v>0.5565019672115644</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2115261851344257</v>
+        <v>0.4820496117075284</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0729396849055774</v>
+        <v>0.2079336009919643</v>
       </c>
       <c r="I6" t="n">
-        <v>0.041777936881408</v>
+        <v>0.1462818918128808</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1502027582377195</v>
+        <v>0.2966689639724791</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3753355480730533</v>
+        <v>0.1924240758332113</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0410893043037503</v>
+        <v>0.2276279454429944</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1660884458106011</v>
+        <v>0.1850130343421673</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0174452075385488</v>
+        <v>0.3284357773760955</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4561439856886863</v>
+        <v>0.745255728562673</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1537583239842206</v>
+        <v>0.2022535077606638</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.1530550580471754</v>
+        <v>0.3284110785461962</v>
       </c>
       <c r="R6" t="n">
-        <v>0.3632830407470465</v>
+        <v>0.3096763979022701</v>
       </c>
       <c r="S6" t="n">
-        <v>0.1600598501041531</v>
+        <v>0.2617676453664899</v>
       </c>
       <c r="T6" t="n">
-        <v>0.6831205785274506</v>
+        <v>0.7718988259633383</v>
       </c>
       <c r="U6" t="n">
-        <v>0.2534121282398701</v>
+        <v>0.5294327323014537</v>
       </c>
       <c r="V6" t="n">
-        <v>0.180814999085851</v>
+        <v>0.4803464661041896</v>
       </c>
       <c r="W6" t="n">
-        <v>0.4921742850914598</v>
+        <v>0.5985923111438751</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>BA 562</t>
+          <t>BA 560</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2304891447226206</v>
+        <v>0.1316252891207114</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7699000636736552</v>
+        <v>0.5403780229389668</v>
       </c>
       <c r="D7" t="n">
-        <v>0.8985457420349121</v>
+        <v>0.377598946611397</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4081504742304484</v>
+        <v>0.4272289484739303</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5565019672115644</v>
+        <v>0.3086892465595156</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4820496117075284</v>
+        <v>0.2115261851344257</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2079336009919643</v>
+        <v>0.0729396849055774</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1462818918128808</v>
+        <v>0.041777936881408</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2966689639724791</v>
+        <v>0.1502027582377195</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1924240758332113</v>
+        <v>0.3753355480730533</v>
       </c>
       <c r="L7" t="n">
-        <v>0.2276279454429944</v>
+        <v>0.0410893043037503</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1850130343421673</v>
+        <v>0.1660884458106011</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3284357773760955</v>
+        <v>0.0174452075385488</v>
       </c>
       <c r="O7" t="n">
-        <v>0.745255728562673</v>
+        <v>0.4561439856886863</v>
       </c>
       <c r="P7" t="n">
-        <v>0.2022535077606638</v>
+        <v>0.1537583239842206</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.3284110785461962</v>
+        <v>0.1530550580471754</v>
       </c>
       <c r="R7" t="n">
-        <v>0.3096763979022701</v>
+        <v>0.3632830407470465</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2617676453664899</v>
+        <v>0.1600598501041531</v>
       </c>
       <c r="T7" t="n">
-        <v>0.7718988259633383</v>
+        <v>0.6831205785274506</v>
       </c>
       <c r="U7" t="n">
-        <v>0.5294327323014537</v>
+        <v>0.2534121282398701</v>
       </c>
       <c r="V7" t="n">
-        <v>0.4803464661041896</v>
+        <v>0.180814999085851</v>
       </c>
       <c r="W7" t="n">
-        <v>0.5985923111438751</v>
+        <v>0.4921742850914598</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>BAEN 502</t>
+          <t>BAEN550B</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.4131923811510205</v>
+        <v>0.6130809113383293</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5705161765217781</v>
+        <v>0.5520257484167814</v>
       </c>
       <c r="D8" t="n">
-        <v>0.4901393800973892</v>
+        <v>0.7207926213741302</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4441793113946914</v>
+        <v>0.505396987311542</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4273738097399473</v>
+        <v>0.5102991163730621</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4605095749720931</v>
+        <v>0.3545858934521675</v>
       </c>
       <c r="H8" t="n">
-        <v>0.2966368296183646</v>
+        <v>0.695765495300293</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1274385708384215</v>
+        <v>0.0186243325006216</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2336553940549492</v>
+        <v>0.0471563602332025</v>
       </c>
       <c r="K8" t="n">
-        <v>0.2568328997585922</v>
+        <v>0.3379862252622843</v>
       </c>
       <c r="L8" t="n">
-        <v>0.3445463813841343</v>
+        <v>0.08517350116744631</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3341414369642734</v>
+        <v>0.0819761119782924</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0706951958127319</v>
+        <v>0.0171027951873838</v>
       </c>
       <c r="O8" t="n">
-        <v>0.5841499026864767</v>
+        <v>0.3302768729627132</v>
       </c>
       <c r="P8" t="n">
-        <v>0.2546422868035733</v>
+        <v>0.3160952031612396</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.6547594703733921</v>
+        <v>0.08563970634713761</v>
       </c>
       <c r="R8" t="n">
-        <v>0.3459584210067987</v>
+        <v>0.6391672128811479</v>
       </c>
       <c r="S8" t="n">
-        <v>0.2995500341057777</v>
+        <v>0.3691503647714853</v>
       </c>
       <c r="T8" t="n">
-        <v>0.654905654489994</v>
+        <v>0.8308229297399521</v>
       </c>
       <c r="U8" t="n">
-        <v>0.294286785647273</v>
+        <v>0.2514807349070906</v>
       </c>
       <c r="V8" t="n">
-        <v>0.6012334153056145</v>
+        <v>0.2023829948157072</v>
       </c>
       <c r="W8" t="n">
-        <v>0.4053647310938686</v>
+        <v>0.1864498648792505</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>BAEN 505</t>
+          <t>BAEN550A</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.419477899144921</v>
+        <v>0.7467707321047783</v>
       </c>
       <c r="C9" t="n">
-        <v>0.5551811622248756</v>
+        <v>0.5111408270895481</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2946426466935211</v>
+        <v>0.862255185842514</v>
       </c>
       <c r="E9" t="n">
-        <v>0.7240229580137465</v>
+        <v>0.4612919702194631</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4410401980082194</v>
+        <v>0.561000756919384</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4939124286174774</v>
+        <v>0.8005906790494919</v>
       </c>
       <c r="H9" t="n">
-        <v>0.7347250762912962</v>
+        <v>0.2602780424058437</v>
       </c>
       <c r="I9" t="n">
-        <v>0.179356709200268</v>
+        <v>0.1804554322734475</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2080965042631659</v>
+        <v>0.1992103946395218</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3532228867212931</v>
+        <v>0.2172507271170616</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1018563462938699</v>
+        <v>0.2725177630782127</v>
       </c>
       <c r="M9" t="n">
-        <v>0.2660307800914678</v>
+        <v>0.2243547989055514</v>
       </c>
       <c r="N9" t="n">
-        <v>0.1156898301948482</v>
+        <v>0.3179881945252418</v>
       </c>
       <c r="O9" t="n">
-        <v>0.5559538801511129</v>
+        <v>0.6328756753355265</v>
       </c>
       <c r="P9" t="n">
-        <v>0.3024969319295552</v>
+        <v>0.3805725993588567</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.2654623041550318</v>
+        <v>0.3892875788733363</v>
       </c>
       <c r="R9" t="n">
-        <v>0.2540673948824405</v>
+        <v>0.414883863646537</v>
       </c>
       <c r="S9" t="n">
-        <v>0.3173346346658137</v>
+        <v>0.6346110180020332</v>
       </c>
       <c r="T9" t="n">
-        <v>0.7251628008153703</v>
+        <v>0.846829354763031</v>
       </c>
       <c r="U9" t="n">
-        <v>0.413664098829031</v>
+        <v>0.5449138432741165</v>
       </c>
       <c r="V9" t="n">
-        <v>0.238883002842259</v>
+        <v>0.5362806580960751</v>
       </c>
       <c r="W9" t="n">
-        <v>0.4775386767254935</v>
+        <v>0.3607520740479231</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>BAEN 506/APSC 541</t>
+          <t>BAEN 549</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6202194858342409</v>
+        <v>0.3619745373725891</v>
       </c>
       <c r="C10" t="n">
-        <v>0.5685641728341579</v>
+        <v>0.5587677049140135</v>
       </c>
       <c r="D10" t="n">
-        <v>0.6860821768641472</v>
+        <v>0.626478374004364</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5972246429882944</v>
+        <v>0.6043004542589188</v>
       </c>
       <c r="F10" t="n">
-        <v>0.4847312700003385</v>
+        <v>0.5602977871894836</v>
       </c>
       <c r="G10" t="n">
-        <v>0.5744984969496727</v>
+        <v>0.6262652575969696</v>
       </c>
       <c r="H10" t="n">
-        <v>0.527806093916297</v>
+        <v>0.1884482130408287</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1257082351366989</v>
+        <v>0.1564639929371575</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2853556517511606</v>
+        <v>0.3069014114638169</v>
       </c>
       <c r="K10" t="n">
-        <v>0.55308254994452</v>
+        <v>0.1539667661612232</v>
       </c>
       <c r="L10" t="n">
-        <v>0.4355110600590706</v>
+        <v>0.2031360877056916</v>
       </c>
       <c r="M10" t="n">
-        <v>0.3126245007297257</v>
+        <v>0.2775002556542555</v>
       </c>
       <c r="N10" t="n">
-        <v>0.1940358420251868</v>
+        <v>0.1084011268491546</v>
       </c>
       <c r="O10" t="n">
-        <v>0.4509221687912941</v>
+        <v>0.8104535440603892</v>
       </c>
       <c r="P10" t="n">
-        <v>0.5125939376302995</v>
+        <v>0.291178452471892</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.6286413616035134</v>
+        <v>0.6579180260499319</v>
       </c>
       <c r="R10" t="n">
-        <v>0.5972891733981669</v>
+        <v>0.1912004038070639</v>
       </c>
       <c r="S10" t="n">
-        <v>0.4842841015197336</v>
+        <v>0.3657821888724963</v>
       </c>
       <c r="T10" t="n">
-        <v>0.8213331177830696</v>
+        <v>0.7895651857058207</v>
       </c>
       <c r="U10" t="n">
-        <v>0.3635560165566858</v>
+        <v>0.6495100756486257</v>
       </c>
       <c r="V10" t="n">
-        <v>0.5955932475626469</v>
+        <v>0.513447180390358</v>
       </c>
       <c r="W10" t="n">
-        <v>0.4822371547343209</v>
+        <v>0.4645010034243266</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>BAEN 509</t>
+          <t>APSC 540</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.5954150427132845</v>
+        <v>0.7273798495531082</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7845326215028763</v>
+        <v>0.8012893199920654</v>
       </c>
       <c r="D11" t="n">
-        <v>0.552040372043848</v>
+        <v>0.8363658785820007</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9092893302440644</v>
+        <v>0.5632544577121734</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5828515887260437</v>
+        <v>0.5751682817935944</v>
       </c>
       <c r="G11" t="n">
-        <v>0.6342340726405382</v>
+        <v>0.6287448763847351</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7842996269464493</v>
+        <v>0.4008272051811218</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0787029343191534</v>
+        <v>0.1901652626693248</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2424858156591653</v>
+        <v>0.247939270734787</v>
       </c>
       <c r="K11" t="n">
-        <v>0.7159931529313326</v>
+        <v>0.5102368395775556</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2045932996552437</v>
+        <v>0.4511112749576568</v>
       </c>
       <c r="M11" t="n">
-        <v>0.2536672875285148</v>
+        <v>0.2955708980560302</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2223373590968549</v>
+        <v>0.2553298756480217</v>
       </c>
       <c r="O11" t="n">
-        <v>0.4832791499793529</v>
+        <v>0.572181236743927</v>
       </c>
       <c r="P11" t="n">
-        <v>0.2928031366318464</v>
+        <v>0.4163009196519852</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.466634901240468</v>
+        <v>0.387138120830059</v>
       </c>
       <c r="R11" t="n">
-        <v>0.4482588768005371</v>
+        <v>0.3014095067977905</v>
       </c>
       <c r="S11" t="n">
-        <v>0.4508405439555645</v>
+        <v>0.403736200928688</v>
       </c>
       <c r="T11" t="n">
-        <v>0.7666752487421036</v>
+        <v>0.8502827048301697</v>
       </c>
       <c r="U11" t="n">
-        <v>0.5238502603024244</v>
+        <v>0.4907763734459877</v>
       </c>
       <c r="V11" t="n">
-        <v>0.5066397227346897</v>
+        <v>0.4016070961952209</v>
       </c>
       <c r="W11" t="n">
-        <v>0.3525203885510564</v>
+        <v>0.5666853606700897</v>
       </c>
     </row>
     <row r="12">
@@ -1357,2191 +1357,2191 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>BAEN 549 (Angele)</t>
+          <t>BASM 516</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.3619745373725891</v>
+        <v>0.3577362075448036</v>
       </c>
       <c r="C13" t="n">
-        <v>0.5587677049140135</v>
+        <v>0.3356479716797669</v>
       </c>
       <c r="D13" t="n">
-        <v>0.626478374004364</v>
+        <v>0.7464047049482664</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6043004542589188</v>
+        <v>0.8093775858481725</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5602977871894836</v>
+        <v>0.5233948354919752</v>
       </c>
       <c r="G13" t="n">
-        <v>0.6262652575969696</v>
+        <v>0.4987799649437268</v>
       </c>
       <c r="H13" t="n">
-        <v>0.1884482130408287</v>
+        <v>0.3553104036448833</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1564639929371575</v>
+        <v>0.06970025356955981</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3069014114638169</v>
+        <v>0.2564774664739768</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1539667661612232</v>
+        <v>0.4446065177520116</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2031360877056916</v>
+        <v>0.5230748156706492</v>
       </c>
       <c r="M13" t="n">
-        <v>0.2775002556542555</v>
+        <v>0.1523610676328341</v>
       </c>
       <c r="N13" t="n">
-        <v>0.1084011268491546</v>
+        <v>0.0218196470135202</v>
       </c>
       <c r="O13" t="n">
-        <v>0.8104535440603892</v>
+        <v>0.6276299556096395</v>
       </c>
       <c r="P13" t="n">
-        <v>0.291178452471892</v>
+        <v>0.2581504826278736</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.6579180260499319</v>
+        <v>0.6620358477036158</v>
       </c>
       <c r="R13" t="n">
-        <v>0.1912004038070639</v>
+        <v>0.5184420372049013</v>
       </c>
       <c r="S13" t="n">
-        <v>0.3657821888724963</v>
+        <v>0.4175791690746943</v>
       </c>
       <c r="T13" t="n">
-        <v>0.7895651857058207</v>
+        <v>0.7626591622829437</v>
       </c>
       <c r="U13" t="n">
-        <v>0.6495100756486257</v>
+        <v>0.316782317434748</v>
       </c>
       <c r="V13" t="n">
-        <v>0.513447180390358</v>
+        <v>0.2911969237029552</v>
       </c>
       <c r="W13" t="n">
-        <v>0.4645010034243266</v>
+        <v>0.5809528008103371</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">BAEN 550 (Angele) - </t>
+          <t>BAEN 509</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.7467707321047783</v>
+        <v>0.5954150427132845</v>
       </c>
       <c r="C14" t="n">
-        <v>0.5111408270895481</v>
+        <v>0.7845326215028763</v>
       </c>
       <c r="D14" t="n">
-        <v>0.862255185842514</v>
+        <v>0.552040372043848</v>
       </c>
       <c r="E14" t="n">
-        <v>0.4612919702194631</v>
+        <v>0.9092893302440644</v>
       </c>
       <c r="F14" t="n">
-        <v>0.561000756919384</v>
+        <v>0.5828515887260437</v>
       </c>
       <c r="G14" t="n">
-        <v>0.8005906790494919</v>
+        <v>0.6342340726405382</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2602780424058437</v>
+        <v>0.7842996269464493</v>
       </c>
       <c r="I14" t="n">
-        <v>0.1804554322734475</v>
+        <v>0.0787029343191534</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1992103946395218</v>
+        <v>0.2424858156591653</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2172507271170616</v>
+        <v>0.7159931529313326</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2725177630782127</v>
+        <v>0.2045932996552437</v>
       </c>
       <c r="M14" t="n">
-        <v>0.2243547989055514</v>
+        <v>0.2536672875285148</v>
       </c>
       <c r="N14" t="n">
-        <v>0.3179881945252418</v>
+        <v>0.2223373590968549</v>
       </c>
       <c r="O14" t="n">
-        <v>0.6328756753355265</v>
+        <v>0.4832791499793529</v>
       </c>
       <c r="P14" t="n">
-        <v>0.3805725993588567</v>
+        <v>0.2928031366318464</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.3892875788733363</v>
+        <v>0.466634901240468</v>
       </c>
       <c r="R14" t="n">
-        <v>0.414883863646537</v>
+        <v>0.4482588768005371</v>
       </c>
       <c r="S14" t="n">
-        <v>0.6346110180020332</v>
+        <v>0.4508405439555645</v>
       </c>
       <c r="T14" t="n">
-        <v>0.846829354763031</v>
+        <v>0.7666752487421036</v>
       </c>
       <c r="U14" t="n">
-        <v>0.5449138432741165</v>
+        <v>0.5238502603024244</v>
       </c>
       <c r="V14" t="n">
-        <v>0.5362806580960751</v>
+        <v>0.5066397227346897</v>
       </c>
       <c r="W14" t="n">
-        <v>0.3607520740479231</v>
+        <v>0.3525203885510564</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>BAEN 550/FCOR 502 (Fraser Pogue)</t>
+          <t>BAEN 506</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.6130809113383293</v>
+        <v>0.6202194858342409</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5520257484167814</v>
+        <v>0.5685641728341579</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7207926213741302</v>
+        <v>0.6860821768641472</v>
       </c>
       <c r="E15" t="n">
-        <v>0.505396987311542</v>
+        <v>0.5972246429882944</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5102991163730621</v>
+        <v>0.4847312700003385</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3545858934521675</v>
+        <v>0.5744984969496727</v>
       </c>
       <c r="H15" t="n">
-        <v>0.695765495300293</v>
+        <v>0.527806093916297</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0186243325006216</v>
+        <v>0.1257082351366989</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0471563602332025</v>
+        <v>0.2853556517511606</v>
       </c>
       <c r="K15" t="n">
-        <v>0.3379862252622843</v>
+        <v>0.55308254994452</v>
       </c>
       <c r="L15" t="n">
-        <v>0.08517350116744631</v>
+        <v>0.4355110600590706</v>
       </c>
       <c r="M15" t="n">
-        <v>0.0819761119782924</v>
+        <v>0.3126245007297257</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0171027951873838</v>
+        <v>0.1940358420251868</v>
       </c>
       <c r="O15" t="n">
-        <v>0.3302768729627132</v>
+        <v>0.4509221687912941</v>
       </c>
       <c r="P15" t="n">
-        <v>0.3160952031612396</v>
+        <v>0.5125939376302995</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.08563970634713761</v>
+        <v>0.6286413616035134</v>
       </c>
       <c r="R15" t="n">
-        <v>0.6391672128811479</v>
+        <v>0.5972891733981669</v>
       </c>
       <c r="S15" t="n">
-        <v>0.3691503647714853</v>
+        <v>0.4842841015197336</v>
       </c>
       <c r="T15" t="n">
-        <v>0.8308229297399521</v>
+        <v>0.8213331177830696</v>
       </c>
       <c r="U15" t="n">
-        <v>0.2514807349070906</v>
+        <v>0.3635560165566858</v>
       </c>
       <c r="V15" t="n">
-        <v>0.2023829948157072</v>
+        <v>0.5955932475626469</v>
       </c>
       <c r="W15" t="n">
-        <v>0.1864498648792505</v>
+        <v>0.4822371547343209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>BAEN 580</t>
+          <t>BAEN 505</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.6776421144604683</v>
+        <v>0.419477899144921</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7572773620486259</v>
+        <v>0.5551811622248756</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8760410100221634</v>
+        <v>0.2946426466935211</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5903653390705585</v>
+        <v>0.7240229580137465</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5230860859155655</v>
+        <v>0.4410401980082194</v>
       </c>
       <c r="G16" t="n">
-        <v>0.6300440952181816</v>
+        <v>0.4939124286174774</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8363740146160126</v>
+        <v>0.7347250762912962</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0790983934421092</v>
+        <v>0.179356709200268</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2010860694572329</v>
+        <v>0.2080965042631659</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4891903721727431</v>
+        <v>0.3532228867212931</v>
       </c>
       <c r="L16" t="n">
-        <v>0.1931973490864038</v>
+        <v>0.1018563462938699</v>
       </c>
       <c r="M16" t="n">
-        <v>0.2247700709849596</v>
+        <v>0.2660307800914678</v>
       </c>
       <c r="N16" t="n">
-        <v>0.2753241355530917</v>
+        <v>0.1156898301948482</v>
       </c>
       <c r="O16" t="n">
-        <v>0.5269269123673439</v>
+        <v>0.5559538801511129</v>
       </c>
       <c r="P16" t="n">
-        <v>0.4770326390862465</v>
+        <v>0.3024969319295552</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.5960461348295212</v>
+        <v>0.2654623041550318</v>
       </c>
       <c r="R16" t="n">
-        <v>0.7274299878627062</v>
+        <v>0.2540673948824405</v>
       </c>
       <c r="S16" t="n">
-        <v>0.5293902922421694</v>
+        <v>0.3173346346658137</v>
       </c>
       <c r="T16" t="n">
-        <v>0.8018344193696976</v>
+        <v>0.7251628008153703</v>
       </c>
       <c r="U16" t="n">
-        <v>0.3202038947492838</v>
+        <v>0.413664098829031</v>
       </c>
       <c r="V16" t="n">
-        <v>0.3311157487332821</v>
+        <v>0.238883002842259</v>
       </c>
       <c r="W16" t="n">
-        <v>0.5707065239548683</v>
+        <v>0.4775386767254935</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>BAEN 580A</t>
+          <t>BAEN 502</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.1834433984414707</v>
+        <v>0.4131923811510205</v>
       </c>
       <c r="C17" t="n">
-        <v>0.413688773555415</v>
+        <v>0.5705161765217781</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3203491995643292</v>
+        <v>0.4901393800973892</v>
       </c>
       <c r="E17" t="n">
-        <v>0.4364164589372064</v>
+        <v>0.4441793113946914</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4117435976596815</v>
+        <v>0.4273738097399473</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2700528663450053</v>
+        <v>0.4605095749720931</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1410570103367458</v>
+        <v>0.2966368296183646</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0620011963016752</v>
+        <v>0.1274385708384215</v>
       </c>
       <c r="J17" t="n">
-        <v>0.07591740660635481</v>
+        <v>0.2336553940549492</v>
       </c>
       <c r="K17" t="n">
-        <v>0.1412378432495253</v>
+        <v>0.2568328997585922</v>
       </c>
       <c r="L17" t="n">
-        <v>0.08231207817776259</v>
+        <v>0.3445463813841343</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2699161336557673</v>
+        <v>0.3341414369642734</v>
       </c>
       <c r="N17" t="n">
-        <v>0.2268037516623735</v>
+        <v>0.0706951958127319</v>
       </c>
       <c r="O17" t="n">
-        <v>0.7226580168519702</v>
+        <v>0.5841499026864767</v>
       </c>
       <c r="P17" t="n">
-        <v>0.2239315990092499</v>
+        <v>0.2546422868035733</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.1580032723556672</v>
+        <v>0.6547594703733921</v>
       </c>
       <c r="R17" t="n">
-        <v>0.4716894509370571</v>
+        <v>0.3459584210067987</v>
       </c>
       <c r="S17" t="n">
-        <v>0.0873092199118608</v>
+        <v>0.2995500341057777</v>
       </c>
       <c r="T17" t="n">
-        <v>0.8163535509790693</v>
+        <v>0.654905654489994</v>
       </c>
       <c r="U17" t="n">
-        <v>0.2775257676839828</v>
+        <v>0.294286785647273</v>
       </c>
       <c r="V17" t="n">
-        <v>0.1430687305733694</v>
+        <v>0.6012334153056145</v>
       </c>
       <c r="W17" t="n">
-        <v>0.314656164497137</v>
+        <v>0.4053647310938686</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>BAEN 580C</t>
+          <t>FCOR 502</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.3066916198780139</v>
+        <v>0.631945937871933</v>
       </c>
       <c r="C18" t="n">
-        <v>0.4349003136157989</v>
+        <v>0.6448477804660797</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2269035100471228</v>
+        <v>0.7779211401939392</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6027461290359497</v>
+        <v>0.5440699011087418</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3717706923683484</v>
+        <v>0.5501353889703751</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2879822670171658</v>
+        <v>0.7292262017726898</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2177003299196561</v>
+        <v>0.2982773035764694</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1489402622682973</v>
+        <v>0.0102671412751078</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2691165028760831</v>
+        <v>0.1930341348052024</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2725043430303533</v>
+        <v>0.2167037464678287</v>
       </c>
       <c r="L18" t="n">
-        <v>0.2392489995885019</v>
+        <v>0.0752856284379959</v>
       </c>
       <c r="M18" t="n">
-        <v>0.1319268185955782</v>
+        <v>0.1995729058980941</v>
       </c>
       <c r="N18" t="n">
-        <v>0.09566769733404119</v>
+        <v>0.3925295751541853</v>
       </c>
       <c r="O18" t="n">
-        <v>0.7304885039726893</v>
+        <v>0.4780744016170501</v>
       </c>
       <c r="P18" t="n">
-        <v>0.3128764902551968</v>
+        <v>0.4120776243507862</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.3300680094398558</v>
+        <v>0.5590949505567551</v>
       </c>
       <c r="R18" t="n">
-        <v>0.3150735727200905</v>
+        <v>0.3549808524549007</v>
       </c>
       <c r="S18" t="n">
-        <v>0.3175627046342318</v>
+        <v>0.4809572100639343</v>
       </c>
       <c r="T18" t="n">
-        <v>0.7339196503162384</v>
+        <v>0.872964471578598</v>
       </c>
       <c r="U18" t="n">
-        <v>0.1526406543950239</v>
+        <v>0.1418165862560272</v>
       </c>
       <c r="V18" t="n">
-        <v>0.2132301593665033</v>
+        <v>0.5163900926709175</v>
       </c>
       <c r="W18" t="n">
-        <v>0.3270305482049783</v>
+        <v>0.4627940058708191</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>BAPA 580</t>
+          <t>COMM 497</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.2472854813871284</v>
+        <v>0.5845940609773</v>
       </c>
       <c r="C19" t="n">
-        <v>0.5908645888169607</v>
+        <v>0.6486443728208542</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3554305862635374</v>
+        <v>0.4664253557566553</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7287373741467794</v>
+        <v>0.582421158750852</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4082688962419827</v>
+        <v>0.3646337812145551</v>
       </c>
       <c r="G19" t="n">
-        <v>0.336679524431626</v>
+        <v>0.3843175694346428</v>
       </c>
       <c r="H19" t="n">
-        <v>0.2482175483213116</v>
+        <v>0.3227461595088243</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2869471477752086</v>
+        <v>0.1401788076618686</v>
       </c>
       <c r="J19" t="n">
-        <v>0.3738296379645665</v>
+        <v>0.2236713779469331</v>
       </c>
       <c r="K19" t="n">
-        <v>0.1793426983058452</v>
+        <v>0.6203844106445709</v>
       </c>
       <c r="L19" t="n">
-        <v>0.2200251342728734</v>
+        <v>0.3389591407030821</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2474037750313679</v>
+        <v>0.2236631903797388</v>
       </c>
       <c r="N19" t="n">
-        <v>0.34411396458745</v>
+        <v>0.2300462659137944</v>
       </c>
       <c r="O19" t="n">
-        <v>0.9326488773028055</v>
+        <v>0.4997575171291828</v>
       </c>
       <c r="P19" t="n">
-        <v>0.1504766469200452</v>
+        <v>0.3315896261483431</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.336603802939256</v>
+        <v>0.2598939103384812</v>
       </c>
       <c r="R19" t="n">
-        <v>0.5664254128932953</v>
+        <v>0.3901915202538172</v>
       </c>
       <c r="S19" t="n">
-        <v>0.2654259722524633</v>
+        <v>0.3170137976606687</v>
       </c>
       <c r="T19" t="n">
-        <v>0.7818077603975931</v>
+        <v>0.607621394097805</v>
       </c>
       <c r="U19" t="n">
-        <v>0.3444054424762726</v>
+        <v>0.2019158935484787</v>
       </c>
       <c r="V19" t="n">
-        <v>0.3947237834023933</v>
+        <v>0.4336782544851303</v>
       </c>
       <c r="W19" t="n">
-        <v>0.0798484074572722</v>
+        <v>0.339182611554861</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>BASM 516</t>
+          <t>COMM 489</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.3577362075448036</v>
+        <v>0.5618747094646096</v>
       </c>
       <c r="C20" t="n">
-        <v>0.3356479716797669</v>
+        <v>0.6658356964588166</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7464047049482664</v>
+        <v>0.4060879207216203</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8093775858481725</v>
+        <v>0.6577599883079529</v>
       </c>
       <c r="F20" t="n">
-        <v>0.5233948354919752</v>
+        <v>0.313611739128828</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4987799649437268</v>
+        <v>0.4889896400272846</v>
       </c>
       <c r="H20" t="n">
-        <v>0.3553104036448833</v>
+        <v>0.6149799644947052</v>
       </c>
       <c r="I20" t="n">
-        <v>0.06970025356955981</v>
+        <v>0.1022287077386863</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2564774664739768</v>
+        <v>0.1156556043773889</v>
       </c>
       <c r="K20" t="n">
-        <v>0.4446065177520116</v>
+        <v>0.6374356001615524</v>
       </c>
       <c r="L20" t="n">
-        <v>0.5230748156706492</v>
+        <v>0.192074461095035</v>
       </c>
       <c r="M20" t="n">
-        <v>0.1523610676328341</v>
+        <v>0.166776093095541</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0218196470135202</v>
+        <v>0.2652115332428366</v>
       </c>
       <c r="O20" t="n">
-        <v>0.6276299556096395</v>
+        <v>0.3669707804918289</v>
       </c>
       <c r="P20" t="n">
-        <v>0.2581504826278736</v>
+        <v>0.262839257903397</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.6620358477036158</v>
+        <v>0.3282323089428246</v>
       </c>
       <c r="R20" t="n">
-        <v>0.5184420372049013</v>
+        <v>0.2906588509678841</v>
       </c>
       <c r="S20" t="n">
-        <v>0.4175791690746943</v>
+        <v>0.4049243916757404</v>
       </c>
       <c r="T20" t="n">
-        <v>0.7626591622829437</v>
+        <v>0.6577278867363929</v>
       </c>
       <c r="U20" t="n">
-        <v>0.316782317434748</v>
+        <v>0.4833767712116241</v>
       </c>
       <c r="V20" t="n">
-        <v>0.2911969237029552</v>
+        <v>0.4668415457010269</v>
       </c>
       <c r="W20" t="n">
-        <v>0.5809528008103371</v>
+        <v>0.2926848486997187</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>BMEG 401</t>
+          <t>APSC 486</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.755716860294342</v>
+        <v>0.5838671823342642</v>
       </c>
       <c r="C21" t="n">
-        <v>0.9293799996376038</v>
+        <v>0.6792886257171631</v>
       </c>
       <c r="D21" t="n">
-        <v>0.6609422564506531</v>
+        <v>0.8493436773618063</v>
       </c>
       <c r="E21" t="n">
-        <v>0.908997356891632</v>
+        <v>0.7451715668042501</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2514711916446686</v>
+        <v>0.6367562015851339</v>
       </c>
       <c r="G21" t="n">
-        <v>0.3311081826686859</v>
+        <v>0.6575605273246765</v>
       </c>
       <c r="H21" t="n">
-        <v>0.8820817470550537</v>
+        <v>0.2406417901317278</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0176207683980464</v>
+        <v>0.22211558263128</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0616597831249237</v>
+        <v>0.2788851782679558</v>
       </c>
       <c r="K21" t="n">
-        <v>0.7681171298027039</v>
+        <v>0.6426869245866934</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2329171299934387</v>
+        <v>0.3509064962466557</v>
       </c>
       <c r="M21" t="n">
-        <v>0.4067531824111938</v>
+        <v>0.3151973485946655</v>
       </c>
       <c r="N21" t="n">
-        <v>0.5430294871330261</v>
+        <v>0.1935244301954905</v>
       </c>
       <c r="O21" t="n">
-        <v>0.8710193634033203</v>
+        <v>0.7736939887205759</v>
       </c>
       <c r="P21" t="n">
-        <v>0.2211381644010543</v>
+        <v>0.3861157620946566</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.7840096354484558</v>
+        <v>0.6769705067078272</v>
       </c>
       <c r="R21" t="n">
-        <v>0.1926587522029876</v>
+        <v>0.5620279088616371</v>
       </c>
       <c r="S21" t="n">
-        <v>0.4659269154071808</v>
+        <v>0.6696630716323853</v>
       </c>
       <c r="T21" t="n">
-        <v>0.6474035382270813</v>
+        <v>0.8885779976844788</v>
       </c>
       <c r="U21" t="n">
-        <v>0.2080147564411163</v>
+        <v>0.2902844001849492</v>
       </c>
       <c r="V21" t="n">
-        <v>0.7239799499511719</v>
+        <v>0.6525993446509043</v>
       </c>
       <c r="W21" t="n">
-        <v>0.1356938183307647</v>
+        <v>0.5568657151112953</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>COMM 280 (101 + 203)</t>
+          <t>COMM 486G</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.7891162782907486</v>
+        <v>0.4641125078002612</v>
       </c>
       <c r="C22" t="n">
-        <v>0.758806400001049</v>
+        <v>0.7022009541591009</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8943345993757248</v>
+        <v>0.6827777059903989</v>
       </c>
       <c r="E22" t="n">
-        <v>0.2799579687416553</v>
+        <v>0.4898923089106877</v>
       </c>
       <c r="F22" t="n">
-        <v>0.627870786935091</v>
+        <v>0.5209588396052519</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5928913690149784</v>
+        <v>0.5845410600304604</v>
       </c>
       <c r="H22" t="n">
-        <v>0.3803380969911814</v>
+        <v>0.1570372295876344</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0600452095095533</v>
+        <v>0.0327471161726862</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0195941788842901</v>
+        <v>0.1834630388766527</v>
       </c>
       <c r="K22" t="n">
-        <v>0.3596942815929651</v>
+        <v>0.1456712756771594</v>
       </c>
       <c r="L22" t="n">
-        <v>0.2925084326416254</v>
+        <v>0.1978818047791719</v>
       </c>
       <c r="M22" t="n">
-        <v>0.1209030855679884</v>
+        <v>0.3887973601619403</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2660374077968299</v>
+        <v>0.1522624545420209</v>
       </c>
       <c r="O22" t="n">
-        <v>0.5604648916050792</v>
+        <v>0.5870461190740267</v>
       </c>
       <c r="P22" t="n">
-        <v>0.3862526910379529</v>
+        <v>0.201222762465477</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.5307759363204241</v>
+        <v>0.4902654985586802</v>
       </c>
       <c r="R22" t="n">
-        <v>0.4327807081863284</v>
+        <v>0.2872850708663463</v>
       </c>
       <c r="S22" t="n">
-        <v>0.5570584610104561</v>
+        <v>0.3783882111310959</v>
       </c>
       <c r="T22" t="n">
-        <v>0.7773628681898117</v>
+        <v>0.7318952791392803</v>
       </c>
       <c r="U22" t="n">
-        <v>0.4182024709880352</v>
+        <v>0.2871163363258044</v>
       </c>
       <c r="V22" t="n">
-        <v>0.4947433127090335</v>
+        <v>0.5533024370670319</v>
       </c>
       <c r="W22" t="n">
-        <v>0.5074924528598785</v>
+        <v>0.304441162229826</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>COMM 280 (102-103/201-202)</t>
+          <t>COMM 485</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.5975096747279167</v>
+        <v>0.1412385924615793</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5183552950620651</v>
+        <v>0.4030936550762918</v>
       </c>
       <c r="D23" t="n">
-        <v>0.6331437174230814</v>
+        <v>0.4674487776226467</v>
       </c>
       <c r="E23" t="n">
-        <v>0.7262365072965622</v>
+        <v>0.2904444858431816</v>
       </c>
       <c r="F23" t="n">
-        <v>0.5175725482404232</v>
+        <v>0.3572150137689378</v>
       </c>
       <c r="G23" t="n">
-        <v>0.5005373060703278</v>
+        <v>0.4054954962597953</v>
       </c>
       <c r="H23" t="n">
-        <v>0.428243663161993</v>
+        <v>0.0485406783668117</v>
       </c>
       <c r="I23" t="n">
-        <v>0.1630647052079439</v>
+        <v>0.032616135250363</v>
       </c>
       <c r="J23" t="n">
-        <v>0.1525838007219135</v>
+        <v>0.0437468868783778</v>
       </c>
       <c r="K23" t="n">
-        <v>0.3718418153002858</v>
+        <v>0.1565625343678726</v>
       </c>
       <c r="L23" t="n">
-        <v>0.2408314682543277</v>
+        <v>0.0748934958957963</v>
       </c>
       <c r="M23" t="n">
-        <v>0.186292028054595</v>
+        <v>0.1828056836707724</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1874798657372594</v>
+        <v>0.2106579293807347</v>
       </c>
       <c r="O23" t="n">
-        <v>0.6006772108376026</v>
+        <v>0.5799254261785083</v>
       </c>
       <c r="P23" t="n">
-        <v>0.2335616573691368</v>
+        <v>0.2493708510365751</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.575586125254631</v>
+        <v>0.1062586938755379</v>
       </c>
       <c r="R23" t="n">
-        <v>0.3860309943556785</v>
+        <v>0.3107936850024594</v>
       </c>
       <c r="S23" t="n">
-        <v>0.2746726106852293</v>
+        <v>0.1018373232541812</v>
       </c>
       <c r="T23" t="n">
-        <v>0.8233945071697235</v>
+        <v>0.6211234364244673</v>
       </c>
       <c r="U23" t="n">
-        <v>0.5052393767982721</v>
+        <v>0.2184515912085771</v>
       </c>
       <c r="V23" t="n">
-        <v>0.4017011753749102</v>
+        <v>0.3667814936488867</v>
       </c>
       <c r="W23" t="n">
-        <v>0.6329867336899042</v>
+        <v>0.1606412670678562</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>COMM 382/COMR 382</t>
+          <t>COMM 482</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.3839674869721586</v>
+        <v>0.341016873717308</v>
       </c>
       <c r="C24" t="n">
-        <v>0.453797040337866</v>
+        <v>0.4556733061456018</v>
       </c>
       <c r="D24" t="n">
-        <v>0.6650111551650546</v>
+        <v>0.3611856492029296</v>
       </c>
       <c r="E24" t="n">
-        <v>0.7609573253853754</v>
+        <v>0.6448673514856232</v>
       </c>
       <c r="F24" t="n">
-        <v>0.5127763084389947</v>
+        <v>0.4817550778388977</v>
       </c>
       <c r="G24" t="n">
-        <v>0.5019962299953807</v>
+        <v>0.3480438904629813</v>
       </c>
       <c r="H24" t="n">
-        <v>0.2396611919287931</v>
+        <v>0.2001770585775375</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1329294021283699</v>
+        <v>0.1331009737526377</v>
       </c>
       <c r="J24" t="n">
-        <v>0.2437568329782648</v>
+        <v>0.2965943755375014</v>
       </c>
       <c r="K24" t="n">
-        <v>0.3662592784755609</v>
+        <v>0.3685221866601043</v>
       </c>
       <c r="L24" t="n">
-        <v>0.3064750283109871</v>
+        <v>0.3459179037147098</v>
       </c>
       <c r="M24" t="n">
-        <v>0.2213663043115626</v>
+        <v>0.1941284967793358</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0789126113946126</v>
+        <v>0.1716647864733305</v>
       </c>
       <c r="O24" t="n">
-        <v>0.6667862602255561</v>
+        <v>0.7382675525214937</v>
       </c>
       <c r="P24" t="n">
-        <v>0.186724330975928</v>
+        <v>0.3531513385888603</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.400908903980797</v>
+        <v>0.2801504039929973</v>
       </c>
       <c r="R24" t="n">
-        <v>0.4222017205743627</v>
+        <v>0.3229825189337134</v>
       </c>
       <c r="S24" t="n">
-        <v>0.4228574762290174</v>
+        <v>0.4100519089649121</v>
       </c>
       <c r="T24" t="n">
-        <v>0.6007216559215025</v>
+        <v>0.584608836306466</v>
       </c>
       <c r="U24" t="n">
-        <v>0.3725810684263706</v>
+        <v>0.3264791404621469</v>
       </c>
       <c r="V24" t="n">
-        <v>0.2967561658641154</v>
+        <v>0.3605230450630188</v>
       </c>
       <c r="W24" t="n">
-        <v>0.5071574854241176</v>
+        <v>0.3426692303684022</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>COMM 383, prev 386D</t>
+          <t>COMM 470</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.2727639134973287</v>
+        <v>0.1736996523104608</v>
       </c>
       <c r="C25" t="n">
-        <v>0.3426586801651865</v>
+        <v>0.4888300821185112</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3506926354020834</v>
+        <v>0.3255444690585136</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5753319002687931</v>
+        <v>0.5904907248914242</v>
       </c>
       <c r="F25" t="n">
-        <v>0.2859746628382709</v>
+        <v>0.3775206506252289</v>
       </c>
       <c r="G25" t="n">
-        <v>0.5717275887727737</v>
+        <v>0.3524769656360149</v>
       </c>
       <c r="H25" t="n">
-        <v>0.1922782862093299</v>
+        <v>0.4030630686320364</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2377602308988571</v>
+        <v>0.1044057188555598</v>
       </c>
       <c r="J25" t="n">
-        <v>0.3474417719990015</v>
+        <v>0.169719498604536</v>
       </c>
       <c r="K25" t="n">
-        <v>0.2650690041482448</v>
+        <v>0.2385038821375928</v>
       </c>
       <c r="L25" t="n">
-        <v>0.228567749261856</v>
+        <v>0.1100860442966222</v>
       </c>
       <c r="M25" t="n">
-        <v>0.2658978141844272</v>
+        <v>0.1780643919482827</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1914404646959155</v>
+        <v>0.2145826043561101</v>
       </c>
       <c r="O25" t="n">
-        <v>0.7182469815015793</v>
+        <v>0.6001475602388382</v>
       </c>
       <c r="P25" t="n">
-        <v>0.3289906652644276</v>
+        <v>0.1825288687832653</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.3800434339791536</v>
+        <v>0.1518111140467226</v>
       </c>
       <c r="R25" t="n">
-        <v>0.3894110368564725</v>
+        <v>0.2133458591997623</v>
       </c>
       <c r="S25" t="n">
-        <v>0.3228924199938774</v>
+        <v>0.161961268633604</v>
       </c>
       <c r="T25" t="n">
-        <v>0.7230709753930569</v>
+        <v>0.7372781410813332</v>
       </c>
       <c r="U25" t="n">
-        <v>0.2952508043963462</v>
+        <v>0.3860626518726349</v>
       </c>
       <c r="V25" t="n">
-        <v>0.3801024220883846</v>
+        <v>0.2140332936542108</v>
       </c>
       <c r="W25" t="n">
-        <v>0.4895532019436359</v>
+        <v>0.3584650419652462</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>COMM 386I</t>
+          <t>COMM 466</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1121145021170377</v>
+        <v>0.5341773947907819</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6073508821427822</v>
+        <v>0.6431275904178619</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3642409311400519</v>
+        <v>0.7527640461921692</v>
       </c>
       <c r="E26" t="n">
-        <v>0.6079207638071643</v>
+        <v>0.6029038710726632</v>
       </c>
       <c r="F26" t="n">
-        <v>0.281076335037748</v>
+        <v>0.517926318777932</v>
       </c>
       <c r="G26" t="n">
-        <v>0.2570505506462521</v>
+        <v>0.5630889038244883</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1930978207124604</v>
+        <v>0.3197547973444064</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0550803345007201</v>
+        <v>0.1048313263389799</v>
       </c>
       <c r="J26" t="n">
-        <v>0.1204207574741707</v>
+        <v>0.1860116401480304</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1571869719870543</v>
+        <v>0.3611805620085861</v>
       </c>
       <c r="L26" t="n">
-        <v>0.1511457736164124</v>
+        <v>0.2436243813070986</v>
       </c>
       <c r="M26" t="n">
-        <v>0.1300020998136865</v>
+        <v>0.2339221864110893</v>
       </c>
       <c r="N26" t="n">
-        <v>0.0525422151032317</v>
+        <v>0.3009017796462608</v>
       </c>
       <c r="O26" t="n">
-        <v>0.6296138163242075</v>
+        <v>0.6659785095188353</v>
       </c>
       <c r="P26" t="n">
-        <v>0.1837126794271171</v>
+        <v>0.3651431587835153</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.1260162294428381</v>
+        <v>0.4761841951145066</v>
       </c>
       <c r="R26" t="n">
-        <v>0.2993900669583429</v>
+        <v>0.4617369464702076</v>
       </c>
       <c r="S26" t="n">
-        <v>0.2041850694869127</v>
+        <v>0.5610646903514862</v>
       </c>
       <c r="T26" t="n">
-        <v>0.6793403393692441</v>
+        <v>0.7887234522236718</v>
       </c>
       <c r="U26" t="n">
-        <v>0.2411139642612801</v>
+        <v>0.2818617158465915</v>
       </c>
       <c r="V26" t="n">
-        <v>0.2229055953212082</v>
+        <v>0.5055244084861543</v>
       </c>
       <c r="W26" t="n">
-        <v>0.134870805137325</v>
+        <v>0.5199402934975095</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>COMM 386L</t>
+          <t>ENPH 459</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.1216019583516754</v>
+        <v>0.1200214028358459</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5545526761561632</v>
+        <v>0.9378277063369752</v>
       </c>
       <c r="D27" t="n">
-        <v>0.2528358111158013</v>
+        <v>0.5820567607879639</v>
       </c>
       <c r="E27" t="n">
-        <v>0.4850943083874881</v>
+        <v>0.4758764505386352</v>
       </c>
       <c r="F27" t="n">
-        <v>0.230796686373651</v>
+        <v>0.5958293080329895</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2804545895196497</v>
+        <v>0.4204452633857727</v>
       </c>
       <c r="H27" t="n">
-        <v>0.2791899447911419</v>
+        <v>0.1376010775566101</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0613975926098646</v>
+        <v>0.0751957595348358</v>
       </c>
       <c r="J27" t="n">
-        <v>0.08971588488202541</v>
+        <v>0.3268598914146423</v>
       </c>
       <c r="K27" t="n">
-        <v>0.219666505116038</v>
+        <v>0.1097597926855087</v>
       </c>
       <c r="L27" t="n">
-        <v>0.0337559729159693</v>
+        <v>0.2098709195852279</v>
       </c>
       <c r="M27" t="n">
-        <v>0.1133702441584318</v>
+        <v>0.2724093198776245</v>
       </c>
       <c r="N27" t="n">
-        <v>0.1008777008100878</v>
+        <v>0.5400866270065308</v>
       </c>
       <c r="O27" t="n">
-        <v>0.4932445008307695</v>
+        <v>0.1286395490169525</v>
       </c>
       <c r="P27" t="n">
-        <v>0.22274896572344</v>
+        <v>0.0492501147091388</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.1871263254724908</v>
+        <v>0.9446349143981934</v>
       </c>
       <c r="R27" t="n">
-        <v>0.20527660229709</v>
+        <v>0.119470901787281</v>
       </c>
       <c r="S27" t="n">
-        <v>0.0850071910535916</v>
+        <v>0.1777084618806839</v>
       </c>
       <c r="T27" t="n">
-        <v>0.6678133420646191</v>
+        <v>0.8447472453117371</v>
       </c>
       <c r="U27" t="n">
-        <v>0.3093091617338359</v>
+        <v>0.7087790966033936</v>
       </c>
       <c r="V27" t="n">
-        <v>0.09520410886034369</v>
+        <v>0.59562748670578</v>
       </c>
       <c r="W27" t="n">
-        <v>0.1362262812908738</v>
+        <v>0.3679929971694946</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>COMM 387/COMR 387/COEC 387</t>
+          <t>DES 445</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.4337684905954769</v>
+        <v>0.9095407128334044</v>
       </c>
       <c r="C28" t="n">
-        <v>0.5638174627508435</v>
+        <v>0.9837970733642578</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5895760314805167</v>
+        <v>0.962541937828064</v>
       </c>
       <c r="E28" t="n">
-        <v>0.8086390580449786</v>
+        <v>0.0399000719189643</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6220221460929939</v>
+        <v>0.5313450694084167</v>
       </c>
       <c r="G28" t="n">
-        <v>0.6107968773160662</v>
+        <v>0.7565801739692688</v>
       </c>
       <c r="H28" t="n">
-        <v>0.6778661140373775</v>
+        <v>0.2102692127227783</v>
       </c>
       <c r="I28" t="n">
-        <v>0.3538890503613012</v>
+        <v>0.0110797015950083</v>
       </c>
       <c r="J28" t="n">
-        <v>0.3044005408883095</v>
+        <v>0.1451659351587295</v>
       </c>
       <c r="K28" t="n">
-        <v>0.4443664412413324</v>
+        <v>0.0379086695611476</v>
       </c>
       <c r="L28" t="n">
-        <v>0.2314278043008276</v>
+        <v>0.1971828937530517</v>
       </c>
       <c r="M28" t="n">
-        <v>0.4345203747174569</v>
+        <v>0.1564930081367492</v>
       </c>
       <c r="N28" t="n">
-        <v>0.4198757010911192</v>
+        <v>0.3347668945789337</v>
       </c>
       <c r="O28" t="n">
-        <v>0.8292113798005241</v>
+        <v>0.1762724220752716</v>
       </c>
       <c r="P28" t="n">
-        <v>0.404174410871097</v>
+        <v>0.09221507608890531</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.4257795895848955</v>
+        <v>0.9791627526283264</v>
       </c>
       <c r="R28" t="n">
-        <v>0.6013223060539791</v>
+        <v>0.0903101414442062</v>
       </c>
       <c r="S28" t="n">
-        <v>0.39162091777793</v>
+        <v>0.6348188519477844</v>
       </c>
       <c r="T28" t="n">
-        <v>0.7676070162228176</v>
+        <v>0.9331275820732116</v>
       </c>
       <c r="U28" t="n">
-        <v>0.5458234788051674</v>
+        <v>0.1318748444318771</v>
       </c>
       <c r="V28" t="n">
-        <v>0.480333160875099</v>
+        <v>0.5010694265365601</v>
       </c>
       <c r="W28" t="n">
-        <v>0.620412996837071</v>
+        <v>0.1725107133388519</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>COMM 389</t>
+          <t>APSC 440</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.2056087525561452</v>
+        <v>0.2606846988201141</v>
       </c>
       <c r="C29" t="n">
-        <v>0.864955261349678</v>
+        <v>0.7093207836151123</v>
       </c>
       <c r="D29" t="n">
-        <v>0.8827962428331375</v>
+        <v>0.513254702091217</v>
       </c>
       <c r="E29" t="n">
-        <v>0.465671441052109</v>
+        <v>0.8721046447753906</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5232194438576698</v>
+        <v>0.185085117816925</v>
       </c>
       <c r="G29" t="n">
-        <v>0.571393609046936</v>
+        <v>0.1172086000442504</v>
       </c>
       <c r="H29" t="n">
-        <v>0.0851247585378587</v>
+        <v>0.0061039207503199</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0976574219530448</v>
+        <v>0.0110382521525025</v>
       </c>
       <c r="J29" t="n">
-        <v>0.294661670923233</v>
+        <v>0.2069031447172165</v>
       </c>
       <c r="K29" t="n">
-        <v>0.2449261960573494</v>
+        <v>0.2184742987155914</v>
       </c>
       <c r="L29" t="n">
-        <v>0.1450743386521935</v>
+        <v>0.5404530763626099</v>
       </c>
       <c r="M29" t="n">
-        <v>0.4392420276999473</v>
+        <v>0.009191735647618699</v>
       </c>
       <c r="N29" t="n">
-        <v>0.4559708310989663</v>
+        <v>0.0219591930508613</v>
       </c>
       <c r="O29" t="n">
-        <v>0.7908002585172653</v>
+        <v>0.8702558279037476</v>
       </c>
       <c r="P29" t="n">
-        <v>0.2934310585260391</v>
+        <v>0.2419787943363189</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.3190620774403214</v>
+        <v>0.9971480369567872</v>
       </c>
       <c r="R29" t="n">
-        <v>0.381632212549448</v>
+        <v>0.4427424073219299</v>
       </c>
       <c r="S29" t="n">
-        <v>0.33427569642663</v>
+        <v>0.5450483560562134</v>
       </c>
       <c r="T29" t="n">
-        <v>0.892446294426918</v>
+        <v>0.5599349141120911</v>
       </c>
       <c r="U29" t="n">
-        <v>0.3310560061363503</v>
+        <v>0.0108648547902703</v>
       </c>
       <c r="V29" t="n">
-        <v>0.5254790922626853</v>
+        <v>0.5322953462600708</v>
       </c>
       <c r="W29" t="n">
-        <v>0.7029887139797211</v>
+        <v>0.0091787232086062</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>COMM 466/APSC486/APSC496A/E  = 2 Term Course</t>
+          <t>BMEG 401</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.5341773947907819</v>
+        <v>0.755716860294342</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6431275904178619</v>
+        <v>0.9293799996376038</v>
       </c>
       <c r="D30" t="n">
-        <v>0.7527640461921692</v>
+        <v>0.6609422564506531</v>
       </c>
       <c r="E30" t="n">
-        <v>0.6029038710726632</v>
+        <v>0.908997356891632</v>
       </c>
       <c r="F30" t="n">
-        <v>0.517926318777932</v>
+        <v>0.2514711916446686</v>
       </c>
       <c r="G30" t="n">
-        <v>0.5630889038244883</v>
+        <v>0.3311081826686859</v>
       </c>
       <c r="H30" t="n">
-        <v>0.3197547973444064</v>
+        <v>0.8820817470550537</v>
       </c>
       <c r="I30" t="n">
-        <v>0.1048313263389799</v>
+        <v>0.0176207683980464</v>
       </c>
       <c r="J30" t="n">
-        <v>0.1860116401480304</v>
+        <v>0.0616597831249237</v>
       </c>
       <c r="K30" t="n">
-        <v>0.3611805620085861</v>
+        <v>0.7681171298027039</v>
       </c>
       <c r="L30" t="n">
-        <v>0.2436243813070986</v>
+        <v>0.2329171299934387</v>
       </c>
       <c r="M30" t="n">
-        <v>0.2339221864110893</v>
+        <v>0.4067531824111938</v>
       </c>
       <c r="N30" t="n">
-        <v>0.3009017796462608</v>
+        <v>0.5430294871330261</v>
       </c>
       <c r="O30" t="n">
-        <v>0.6659785095188353</v>
+        <v>0.8710193634033203</v>
       </c>
       <c r="P30" t="n">
-        <v>0.3651431587835153</v>
+        <v>0.2211381644010543</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.4761841951145066</v>
+        <v>0.7840096354484558</v>
       </c>
       <c r="R30" t="n">
-        <v>0.4617369464702076</v>
+        <v>0.1926587522029876</v>
       </c>
       <c r="S30" t="n">
-        <v>0.5610646903514862</v>
+        <v>0.4659269154071808</v>
       </c>
       <c r="T30" t="n">
-        <v>0.7887234522236718</v>
+        <v>0.6474035382270813</v>
       </c>
       <c r="U30" t="n">
-        <v>0.2818617158465915</v>
+        <v>0.2080147564411163</v>
       </c>
       <c r="V30" t="n">
-        <v>0.5055244084861543</v>
+        <v>0.7239799499511719</v>
       </c>
       <c r="W30" t="n">
-        <v>0.5199402934975095</v>
+        <v>0.1356938183307647</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>COMM 470</t>
+          <t>COMM 389</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.1736996523104608</v>
+        <v>0.2056087525561452</v>
       </c>
       <c r="C31" t="n">
-        <v>0.4888300821185112</v>
+        <v>0.864955261349678</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3255444690585136</v>
+        <v>0.8827962428331375</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5904907248914242</v>
+        <v>0.465671441052109</v>
       </c>
       <c r="F31" t="n">
-        <v>0.3775206506252289</v>
+        <v>0.5232194438576698</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3524769656360149</v>
+        <v>0.571393609046936</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4030630686320364</v>
+        <v>0.0851247585378587</v>
       </c>
       <c r="I31" t="n">
-        <v>0.1044057188555598</v>
+        <v>0.0976574219530448</v>
       </c>
       <c r="J31" t="n">
-        <v>0.169719498604536</v>
+        <v>0.294661670923233</v>
       </c>
       <c r="K31" t="n">
-        <v>0.2385038821375928</v>
+        <v>0.2449261960573494</v>
       </c>
       <c r="L31" t="n">
-        <v>0.1100860442966222</v>
+        <v>0.1450743386521935</v>
       </c>
       <c r="M31" t="n">
-        <v>0.1780643919482827</v>
+        <v>0.4392420276999473</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2145826043561101</v>
+        <v>0.4559708310989663</v>
       </c>
       <c r="O31" t="n">
-        <v>0.6001475602388382</v>
+        <v>0.7908002585172653</v>
       </c>
       <c r="P31" t="n">
-        <v>0.1825288687832653</v>
+        <v>0.2934310585260391</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.1518111140467226</v>
+        <v>0.3190620774403214</v>
       </c>
       <c r="R31" t="n">
-        <v>0.2133458591997623</v>
+        <v>0.381632212549448</v>
       </c>
       <c r="S31" t="n">
-        <v>0.161961268633604</v>
+        <v>0.33427569642663</v>
       </c>
       <c r="T31" t="n">
-        <v>0.7372781410813332</v>
+        <v>0.892446294426918</v>
       </c>
       <c r="U31" t="n">
-        <v>0.3860626518726349</v>
+        <v>0.3310560061363503</v>
       </c>
       <c r="V31" t="n">
-        <v>0.2140332936542108</v>
+        <v>0.5254790922626853</v>
       </c>
       <c r="W31" t="n">
-        <v>0.3584650419652462</v>
+        <v>0.7029887139797211</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>COMM 482 / BAMA 503 001</t>
+          <t>COMM 388</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.341016873717308</v>
+        <v>0.336957287043333</v>
       </c>
       <c r="C32" t="n">
-        <v>0.4556733061456018</v>
+        <v>0.6510748416185379</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3611856492029296</v>
+        <v>0.7205885456351098</v>
       </c>
       <c r="E32" t="n">
-        <v>0.6448673514856232</v>
+        <v>0.62085978128016</v>
       </c>
       <c r="F32" t="n">
-        <v>0.4817550778388977</v>
+        <v>0.620234887348488</v>
       </c>
       <c r="G32" t="n">
-        <v>0.3480438904629813</v>
+        <v>0.5600260645151138</v>
       </c>
       <c r="H32" t="n">
-        <v>0.2001770585775375</v>
+        <v>0.1951600573956966</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1331009737526377</v>
+        <v>0.1367978537455201</v>
       </c>
       <c r="J32" t="n">
-        <v>0.2965943755375014</v>
+        <v>0.4575793892145157</v>
       </c>
       <c r="K32" t="n">
-        <v>0.3685221866601043</v>
+        <v>0.2201638254337012</v>
       </c>
       <c r="L32" t="n">
-        <v>0.3459179037147098</v>
+        <v>0.2302085999399423</v>
       </c>
       <c r="M32" t="n">
-        <v>0.1941284967793358</v>
+        <v>0.6777667477726936</v>
       </c>
       <c r="N32" t="n">
-        <v>0.1716647864733305</v>
+        <v>0.3489179639145732</v>
       </c>
       <c r="O32" t="n">
-        <v>0.7382675525214937</v>
+        <v>0.5475482884794474</v>
       </c>
       <c r="P32" t="n">
-        <v>0.3531513385888603</v>
+        <v>0.2899648696184158</v>
       </c>
       <c r="Q32" t="n">
-        <v>0.2801504039929973</v>
+        <v>0.4951174184679985</v>
       </c>
       <c r="R32" t="n">
-        <v>0.3229825189337134</v>
+        <v>0.7259702980518341</v>
       </c>
       <c r="S32" t="n">
-        <v>0.4100519089649121</v>
+        <v>0.412698432803154</v>
       </c>
       <c r="T32" t="n">
-        <v>0.584608836306466</v>
+        <v>0.838713750243187</v>
       </c>
       <c r="U32" t="n">
-        <v>0.3264791404621469</v>
+        <v>0.09822934796102339</v>
       </c>
       <c r="V32" t="n">
-        <v>0.3605230450630188</v>
+        <v>0.7390108928084373</v>
       </c>
       <c r="W32" t="n">
-        <v>0.3426692303684022</v>
+        <v>0.4098045746795833</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>COMM 485</t>
+          <t>COMM 387</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.1412385924615793</v>
+        <v>0.4337684905954769</v>
       </c>
       <c r="C33" t="n">
-        <v>0.4030936550762918</v>
+        <v>0.5638174627508435</v>
       </c>
       <c r="D33" t="n">
-        <v>0.4674487776226467</v>
+        <v>0.5895760314805167</v>
       </c>
       <c r="E33" t="n">
-        <v>0.2904444858431816</v>
+        <v>0.8086390580449786</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3572150137689378</v>
+        <v>0.6220221460929939</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4054954962597953</v>
+        <v>0.6107968773160662</v>
       </c>
       <c r="H33" t="n">
-        <v>0.0485406783668117</v>
+        <v>0.6778661140373775</v>
       </c>
       <c r="I33" t="n">
-        <v>0.032616135250363</v>
+        <v>0.3538890503613012</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0437468868783778</v>
+        <v>0.3044005408883095</v>
       </c>
       <c r="K33" t="n">
-        <v>0.1565625343678726</v>
+        <v>0.4443664412413324</v>
       </c>
       <c r="L33" t="n">
-        <v>0.0748934958957963</v>
+        <v>0.2314278043008276</v>
       </c>
       <c r="M33" t="n">
-        <v>0.1828056836707724</v>
+        <v>0.4345203747174569</v>
       </c>
       <c r="N33" t="n">
-        <v>0.2106579293807347</v>
+        <v>0.4198757010911192</v>
       </c>
       <c r="O33" t="n">
-        <v>0.5799254261785083</v>
+        <v>0.8292113798005241</v>
       </c>
       <c r="P33" t="n">
-        <v>0.2493708510365751</v>
+        <v>0.404174410871097</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.1062586938755379</v>
+        <v>0.4257795895848955</v>
       </c>
       <c r="R33" t="n">
-        <v>0.3107936850024594</v>
+        <v>0.6013223060539791</v>
       </c>
       <c r="S33" t="n">
-        <v>0.1018373232541812</v>
+        <v>0.39162091777793</v>
       </c>
       <c r="T33" t="n">
-        <v>0.6211234364244673</v>
+        <v>0.7676070162228176</v>
       </c>
       <c r="U33" t="n">
-        <v>0.2184515912085771</v>
+        <v>0.5458234788051674</v>
       </c>
       <c r="V33" t="n">
-        <v>0.3667814936488867</v>
+        <v>0.480333160875099</v>
       </c>
       <c r="W33" t="n">
-        <v>0.1606412670678562</v>
+        <v>0.620412996837071</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>COMM 486G / BAEN 510</t>
+          <t>COMM 386L</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.4641125078002612</v>
+        <v>0.1216019583516754</v>
       </c>
       <c r="C34" t="n">
-        <v>0.7022009541591009</v>
+        <v>0.5545526761561632</v>
       </c>
       <c r="D34" t="n">
-        <v>0.6827777059903989</v>
+        <v>0.2528358111158013</v>
       </c>
       <c r="E34" t="n">
-        <v>0.4898923089106877</v>
+        <v>0.4850943083874881</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5209588396052519</v>
+        <v>0.230796686373651</v>
       </c>
       <c r="G34" t="n">
-        <v>0.5845410600304604</v>
+        <v>0.2804545895196497</v>
       </c>
       <c r="H34" t="n">
-        <v>0.1570372295876344</v>
+        <v>0.2791899447911419</v>
       </c>
       <c r="I34" t="n">
-        <v>0.0327471161726862</v>
+        <v>0.0613975926098646</v>
       </c>
       <c r="J34" t="n">
-        <v>0.1834630388766527</v>
+        <v>0.08971588488202541</v>
       </c>
       <c r="K34" t="n">
-        <v>0.1456712756771594</v>
+        <v>0.219666505116038</v>
       </c>
       <c r="L34" t="n">
-        <v>0.1978818047791719</v>
+        <v>0.0337559729159693</v>
       </c>
       <c r="M34" t="n">
-        <v>0.3887973601619403</v>
+        <v>0.1133702441584318</v>
       </c>
       <c r="N34" t="n">
-        <v>0.1522624545420209</v>
+        <v>0.1008777008100878</v>
       </c>
       <c r="O34" t="n">
-        <v>0.5870461190740267</v>
+        <v>0.4932445008307695</v>
       </c>
       <c r="P34" t="n">
-        <v>0.201222762465477</v>
+        <v>0.22274896572344</v>
       </c>
       <c r="Q34" t="n">
-        <v>0.4902654985586802</v>
+        <v>0.1871263254724908</v>
       </c>
       <c r="R34" t="n">
-        <v>0.2872850708663463</v>
+        <v>0.20527660229709</v>
       </c>
       <c r="S34" t="n">
-        <v>0.3783882111310959</v>
+        <v>0.0850071910535916</v>
       </c>
       <c r="T34" t="n">
-        <v>0.7318952791392803</v>
+        <v>0.6678133420646191</v>
       </c>
       <c r="U34" t="n">
-        <v>0.2871163363258044</v>
+        <v>0.3093091617338359</v>
       </c>
       <c r="V34" t="n">
-        <v>0.5533024370670319</v>
+        <v>0.09520410886034369</v>
       </c>
       <c r="W34" t="n">
-        <v>0.304441162229826</v>
+        <v>0.1362262812908738</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>COMM 489</t>
+          <t>COMM 386I</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.5618747094646096</v>
+        <v>0.1121145021170377</v>
       </c>
       <c r="C35" t="n">
-        <v>0.6658356964588166</v>
+        <v>0.6073508821427822</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4060879207216203</v>
+        <v>0.3642409311400519</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6577599883079529</v>
+        <v>0.6079207638071643</v>
       </c>
       <c r="F35" t="n">
-        <v>0.313611739128828</v>
+        <v>0.281076335037748</v>
       </c>
       <c r="G35" t="n">
-        <v>0.4889896400272846</v>
+        <v>0.2570505506462521</v>
       </c>
       <c r="H35" t="n">
-        <v>0.6149799644947052</v>
+        <v>0.1930978207124604</v>
       </c>
       <c r="I35" t="n">
-        <v>0.1022287077386863</v>
+        <v>0.0550803345007201</v>
       </c>
       <c r="J35" t="n">
-        <v>0.1156556043773889</v>
+        <v>0.1204207574741707</v>
       </c>
       <c r="K35" t="n">
-        <v>0.6374356001615524</v>
+        <v>0.1571869719870543</v>
       </c>
       <c r="L35" t="n">
-        <v>0.192074461095035</v>
+        <v>0.1511457736164124</v>
       </c>
       <c r="M35" t="n">
-        <v>0.166776093095541</v>
+        <v>0.1300020998136865</v>
       </c>
       <c r="N35" t="n">
-        <v>0.2652115332428366</v>
+        <v>0.0525422151032317</v>
       </c>
       <c r="O35" t="n">
-        <v>0.3669707804918289</v>
+        <v>0.6296138163242075</v>
       </c>
       <c r="P35" t="n">
-        <v>0.262839257903397</v>
+        <v>0.1837126794271171</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.3282323089428246</v>
+        <v>0.1260162294428381</v>
       </c>
       <c r="R35" t="n">
-        <v>0.2906588509678841</v>
+        <v>0.2993900669583429</v>
       </c>
       <c r="S35" t="n">
-        <v>0.4049243916757404</v>
+        <v>0.2041850694869127</v>
       </c>
       <c r="T35" t="n">
-        <v>0.6577278867363929</v>
+        <v>0.6793403393692441</v>
       </c>
       <c r="U35" t="n">
-        <v>0.4833767712116241</v>
+        <v>0.2411139642612801</v>
       </c>
       <c r="V35" t="n">
-        <v>0.4668415457010269</v>
+        <v>0.2229055953212082</v>
       </c>
       <c r="W35" t="n">
-        <v>0.2926848486997187</v>
+        <v>0.134870805137325</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>COMM 497/  COMR 497</t>
+          <t>COMM 383</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.5845940609773</v>
+        <v>0.2727639134973287</v>
       </c>
       <c r="C36" t="n">
-        <v>0.6486443728208542</v>
+        <v>0.3426586801651865</v>
       </c>
       <c r="D36" t="n">
-        <v>0.4664253557566553</v>
+        <v>0.3506926354020834</v>
       </c>
       <c r="E36" t="n">
-        <v>0.582421158750852</v>
+        <v>0.5753319002687931</v>
       </c>
       <c r="F36" t="n">
-        <v>0.3646337812145551</v>
+        <v>0.2859746628382709</v>
       </c>
       <c r="G36" t="n">
-        <v>0.3843175694346428</v>
+        <v>0.5717275887727737</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3227461595088243</v>
+        <v>0.1922782862093299</v>
       </c>
       <c r="I36" t="n">
-        <v>0.1401788076618686</v>
+        <v>0.2377602308988571</v>
       </c>
       <c r="J36" t="n">
-        <v>0.2236713779469331</v>
+        <v>0.3474417719990015</v>
       </c>
       <c r="K36" t="n">
-        <v>0.6203844106445709</v>
+        <v>0.2650690041482448</v>
       </c>
       <c r="L36" t="n">
-        <v>0.3389591407030821</v>
+        <v>0.228567749261856</v>
       </c>
       <c r="M36" t="n">
-        <v>0.2236631903797388</v>
+        <v>0.2658978141844272</v>
       </c>
       <c r="N36" t="n">
-        <v>0.2300462659137944</v>
+        <v>0.1914404646959155</v>
       </c>
       <c r="O36" t="n">
-        <v>0.4997575171291828</v>
+        <v>0.7182469815015793</v>
       </c>
       <c r="P36" t="n">
-        <v>0.3315896261483431</v>
+        <v>0.3289906652644276</v>
       </c>
       <c r="Q36" t="n">
-        <v>0.2598939103384812</v>
+        <v>0.3800434339791536</v>
       </c>
       <c r="R36" t="n">
-        <v>0.3901915202538172</v>
+        <v>0.3894110368564725</v>
       </c>
       <c r="S36" t="n">
-        <v>0.3170137976606687</v>
+        <v>0.3228924199938774</v>
       </c>
       <c r="T36" t="n">
-        <v>0.607621394097805</v>
+        <v>0.7230709753930569</v>
       </c>
       <c r="U36" t="n">
-        <v>0.2019158935484787</v>
+        <v>0.2952508043963462</v>
       </c>
       <c r="V36" t="n">
-        <v>0.4336782544851303</v>
+        <v>0.3801024220883846</v>
       </c>
       <c r="W36" t="n">
-        <v>0.339182611554861</v>
+        <v>0.4895532019436359</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>COMM/COMR 388</t>
+          <t>APSC 383</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.336957287043333</v>
+        <v>0.225077636539936</v>
       </c>
       <c r="C37" t="n">
-        <v>0.6510748416185379</v>
+        <v>0.6893610060214996</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7205885456351098</v>
+        <v>0.5513069182634354</v>
       </c>
       <c r="E37" t="n">
-        <v>0.62085978128016</v>
+        <v>0.4186507612466812</v>
       </c>
       <c r="F37" t="n">
-        <v>0.620234887348488</v>
+        <v>0.3057575821876526</v>
       </c>
       <c r="G37" t="n">
-        <v>0.5600260645151138</v>
+        <v>0.4233366549015045</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1951600573956966</v>
+        <v>0.1879539787769317</v>
       </c>
       <c r="I37" t="n">
-        <v>0.1367978537455201</v>
+        <v>0.0409446209669113</v>
       </c>
       <c r="J37" t="n">
-        <v>0.4575793892145157</v>
+        <v>0.1995269060134887</v>
       </c>
       <c r="K37" t="n">
-        <v>0.2201638254337012</v>
+        <v>0.1937873214483261</v>
       </c>
       <c r="L37" t="n">
-        <v>0.2302085999399423</v>
+        <v>0.2508588880300522</v>
       </c>
       <c r="M37" t="n">
-        <v>0.6777667477726936</v>
+        <v>0.1923822909593582</v>
       </c>
       <c r="N37" t="n">
-        <v>0.3489179639145732</v>
+        <v>0.4476391971111297</v>
       </c>
       <c r="O37" t="n">
-        <v>0.5475482884794474</v>
+        <v>0.5635110065340996</v>
       </c>
       <c r="P37" t="n">
-        <v>0.2899648696184158</v>
+        <v>0.2413162365555763</v>
       </c>
       <c r="Q37" t="n">
-        <v>0.4951174184679985</v>
+        <v>0.2752360552549362</v>
       </c>
       <c r="R37" t="n">
-        <v>0.7259702980518341</v>
+        <v>0.2399156466126442</v>
       </c>
       <c r="S37" t="n">
-        <v>0.412698432803154</v>
+        <v>0.519437164068222</v>
       </c>
       <c r="T37" t="n">
-        <v>0.838713750243187</v>
+        <v>0.6512212306261063</v>
       </c>
       <c r="U37" t="n">
-        <v>0.09822934796102339</v>
+        <v>0.0901582948863506</v>
       </c>
       <c r="V37" t="n">
-        <v>0.7390108928084373</v>
+        <v>0.4331253916025162</v>
       </c>
       <c r="W37" t="n">
-        <v>0.4098045746795833</v>
+        <v>0.5061413943767548</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>COMR 280</t>
+          <t>COMM 382</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.7031998038291931</v>
+        <v>0.3839674869721586</v>
       </c>
       <c r="C38" t="n">
-        <v>0.7241581678390503</v>
+        <v>0.453797040337866</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8025444746017456</v>
+        <v>0.6650111551650546</v>
       </c>
       <c r="E38" t="n">
-        <v>0.7870652079582214</v>
+        <v>0.7609573253853754</v>
       </c>
       <c r="F38" t="n">
-        <v>0.5450968742370605</v>
+        <v>0.5127763084389947</v>
       </c>
       <c r="G38" t="n">
-        <v>0.7926843166351318</v>
+        <v>0.5019962299953807</v>
       </c>
       <c r="H38" t="n">
-        <v>0.1099151894450187</v>
+        <v>0.2396611919287931</v>
       </c>
       <c r="I38" t="n">
-        <v>0.07564053684473029</v>
+        <v>0.1329294021283699</v>
       </c>
       <c r="J38" t="n">
-        <v>0.0209463313221931</v>
+        <v>0.2437568329782648</v>
       </c>
       <c r="K38" t="n">
-        <v>0.1921039819717407</v>
+        <v>0.3662592784755609</v>
       </c>
       <c r="L38" t="n">
-        <v>0.18061164021492</v>
+        <v>0.3064750283109871</v>
       </c>
       <c r="M38" t="n">
-        <v>0.2662175297737121</v>
+        <v>0.2213663043115626</v>
       </c>
       <c r="N38" t="n">
-        <v>0.1900261491537094</v>
+        <v>0.0789126113946126</v>
       </c>
       <c r="O38" t="n">
-        <v>0.9560589790344238</v>
+        <v>0.6667862602255561</v>
       </c>
       <c r="P38" t="n">
-        <v>0.9059367179870604</v>
+        <v>0.186724330975928</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.976838231086731</v>
+        <v>0.400908903980797</v>
       </c>
       <c r="R38" t="n">
-        <v>0.9503455758094788</v>
+        <v>0.4222017205743627</v>
       </c>
       <c r="S38" t="n">
-        <v>0.595852792263031</v>
+        <v>0.4228574762290174</v>
       </c>
       <c r="T38" t="n">
-        <v>0.820959746837616</v>
+        <v>0.6007216559215025</v>
       </c>
       <c r="U38" t="n">
-        <v>0.8192307949066162</v>
+        <v>0.3725810684263706</v>
       </c>
       <c r="V38" t="n">
-        <v>0.1808323711156845</v>
+        <v>0.2967561658641154</v>
       </c>
       <c r="W38" t="n">
-        <v>0.6900633573532104</v>
+        <v>0.5071574854241176</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>DES 445</t>
+          <t>IGEN 340</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.9095407128334044</v>
+        <v>0.7891162782907486</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9837970733642578</v>
+        <v>0.758806400001049</v>
       </c>
       <c r="D39" t="n">
-        <v>0.962541937828064</v>
+        <v>0.8943345993757248</v>
       </c>
       <c r="E39" t="n">
-        <v>0.0399000719189643</v>
+        <v>0.2799579687416553</v>
       </c>
       <c r="F39" t="n">
-        <v>0.5313450694084167</v>
+        <v>0.627870786935091</v>
       </c>
       <c r="G39" t="n">
-        <v>0.7565801739692688</v>
+        <v>0.5928913690149784</v>
       </c>
       <c r="H39" t="n">
-        <v>0.2102692127227783</v>
+        <v>0.3803380969911814</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0110797015950083</v>
+        <v>0.0600452095095533</v>
       </c>
       <c r="J39" t="n">
-        <v>0.1451659351587295</v>
+        <v>0.0195941788842901</v>
       </c>
       <c r="K39" t="n">
-        <v>0.0379086695611476</v>
+        <v>0.3596942815929651</v>
       </c>
       <c r="L39" t="n">
-        <v>0.1971828937530517</v>
+        <v>0.2925084326416254</v>
       </c>
       <c r="M39" t="n">
-        <v>0.1564930081367492</v>
+        <v>0.1209030855679884</v>
       </c>
       <c r="N39" t="n">
-        <v>0.3347668945789337</v>
+        <v>0.2660374077968299</v>
       </c>
       <c r="O39" t="n">
-        <v>0.1762724220752716</v>
+        <v>0.5604648916050792</v>
       </c>
       <c r="P39" t="n">
-        <v>0.09221507608890531</v>
+        <v>0.3862526910379529</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.9791627526283264</v>
+        <v>0.5307759363204241</v>
       </c>
       <c r="R39" t="n">
-        <v>0.0903101414442062</v>
+        <v>0.4327807081863284</v>
       </c>
       <c r="S39" t="n">
-        <v>0.6348188519477844</v>
+        <v>0.5570584610104561</v>
       </c>
       <c r="T39" t="n">
-        <v>0.9331275820732116</v>
+        <v>0.7773628681898117</v>
       </c>
       <c r="U39" t="n">
-        <v>0.1318748444318771</v>
+        <v>0.4182024709880352</v>
       </c>
       <c r="V39" t="n">
-        <v>0.5010694265365601</v>
+        <v>0.4947433127090335</v>
       </c>
       <c r="W39" t="n">
-        <v>0.1725107133388519</v>
+        <v>0.5074924528598785</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>ENPH 459 &amp; 479</t>
+          <t>COMR 280</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.1200214028358459</v>
+        <v>0.7031998038291931</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9378277063369752</v>
+        <v>0.7241581678390503</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5820567607879639</v>
+        <v>0.8025444746017456</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4758764505386352</v>
+        <v>0.7870652079582214</v>
       </c>
       <c r="F40" t="n">
-        <v>0.5958293080329895</v>
+        <v>0.5450968742370605</v>
       </c>
       <c r="G40" t="n">
-        <v>0.4204452633857727</v>
+        <v>0.7926843166351318</v>
       </c>
       <c r="H40" t="n">
-        <v>0.1376010775566101</v>
+        <v>0.1099151894450187</v>
       </c>
       <c r="I40" t="n">
-        <v>0.0751957595348358</v>
+        <v>0.07564053684473029</v>
       </c>
       <c r="J40" t="n">
-        <v>0.3268598914146423</v>
+        <v>0.0209463313221931</v>
       </c>
       <c r="K40" t="n">
-        <v>0.1097597926855087</v>
+        <v>0.1921039819717407</v>
       </c>
       <c r="L40" t="n">
-        <v>0.2098709195852279</v>
+        <v>0.18061164021492</v>
       </c>
       <c r="M40" t="n">
-        <v>0.2724093198776245</v>
+        <v>0.2662175297737121</v>
       </c>
       <c r="N40" t="n">
-        <v>0.5400866270065308</v>
+        <v>0.1900261491537094</v>
       </c>
       <c r="O40" t="n">
-        <v>0.1286395490169525</v>
+        <v>0.9560589790344238</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0492501147091388</v>
+        <v>0.9059367179870604</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.9446349143981934</v>
+        <v>0.976838231086731</v>
       </c>
       <c r="R40" t="n">
-        <v>0.119470901787281</v>
+        <v>0.9503455758094788</v>
       </c>
       <c r="S40" t="n">
-        <v>0.1777084618806839</v>
+        <v>0.595852792263031</v>
       </c>
       <c r="T40" t="n">
-        <v>0.8447472453117371</v>
+        <v>0.820959746837616</v>
       </c>
       <c r="U40" t="n">
-        <v>0.7087790966033936</v>
+        <v>0.8192307949066162</v>
       </c>
       <c r="V40" t="n">
-        <v>0.59562748670578</v>
+        <v>0.1808323711156845</v>
       </c>
       <c r="W40" t="n">
-        <v>0.3679929971694946</v>
+        <v>0.6900633573532104</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>FCOR 502</t>
+          <t>COMM 280B</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.631945937871933</v>
+        <v>0.7891162782907486</v>
       </c>
       <c r="C41" t="n">
-        <v>0.6448477804660797</v>
+        <v>0.758806400001049</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7779211401939392</v>
+        <v>0.8943345993757248</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5440699011087418</v>
+        <v>0.2799579687416553</v>
       </c>
       <c r="F41" t="n">
-        <v>0.5501353889703751</v>
+        <v>0.627870786935091</v>
       </c>
       <c r="G41" t="n">
-        <v>0.7292262017726898</v>
+        <v>0.5928913690149784</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2982773035764694</v>
+        <v>0.3803380969911814</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0102671412751078</v>
+        <v>0.0600452095095533</v>
       </c>
       <c r="J41" t="n">
-        <v>0.1930341348052024</v>
+        <v>0.0195941788842901</v>
       </c>
       <c r="K41" t="n">
-        <v>0.2167037464678287</v>
+        <v>0.3596942815929651</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0752856284379959</v>
+        <v>0.2925084326416254</v>
       </c>
       <c r="M41" t="n">
-        <v>0.1995729058980941</v>
+        <v>0.1209030855679884</v>
       </c>
       <c r="N41" t="n">
-        <v>0.3925295751541853</v>
+        <v>0.2660374077968299</v>
       </c>
       <c r="O41" t="n">
-        <v>0.4780744016170501</v>
+        <v>0.5604648916050792</v>
       </c>
       <c r="P41" t="n">
-        <v>0.4120776243507862</v>
+        <v>0.3862526910379529</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.5590949505567551</v>
+        <v>0.5307759363204241</v>
       </c>
       <c r="R41" t="n">
-        <v>0.3549808524549007</v>
+        <v>0.4327807081863284</v>
       </c>
       <c r="S41" t="n">
-        <v>0.4809572100639343</v>
+        <v>0.5570584610104561</v>
       </c>
       <c r="T41" t="n">
-        <v>0.872964471578598</v>
+        <v>0.7773628681898117</v>
       </c>
       <c r="U41" t="n">
-        <v>0.1418165862560272</v>
+        <v>0.4182024709880352</v>
       </c>
       <c r="V41" t="n">
-        <v>0.5163900926709175</v>
+        <v>0.4947433127090335</v>
       </c>
       <c r="W41" t="n">
-        <v>0.4627940058708191</v>
+        <v>0.5074924528598785</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>IGEN 340</t>
+          <t>COMM 280A</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.7891162782907486</v>
+        <v>0.5975096747279167</v>
       </c>
       <c r="C42" t="n">
-        <v>0.758806400001049</v>
+        <v>0.5183552950620651</v>
       </c>
       <c r="D42" t="n">
-        <v>0.8943345993757248</v>
+        <v>0.6331437174230814</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2799579687416553</v>
+        <v>0.7262365072965622</v>
       </c>
       <c r="F42" t="n">
-        <v>0.627870786935091</v>
+        <v>0.5175725482404232</v>
       </c>
       <c r="G42" t="n">
-        <v>0.5928913690149784</v>
+        <v>0.5005373060703278</v>
       </c>
       <c r="H42" t="n">
-        <v>0.3803380969911814</v>
+        <v>0.428243663161993</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0600452095095533</v>
+        <v>0.1630647052079439</v>
       </c>
       <c r="J42" t="n">
-        <v>0.0195941788842901</v>
+        <v>0.1525838007219135</v>
       </c>
       <c r="K42" t="n">
-        <v>0.3596942815929651</v>
+        <v>0.3718418153002858</v>
       </c>
       <c r="L42" t="n">
-        <v>0.2925084326416254</v>
+        <v>0.2408314682543277</v>
       </c>
       <c r="M42" t="n">
-        <v>0.1209030855679884</v>
+        <v>0.186292028054595</v>
       </c>
       <c r="N42" t="n">
-        <v>0.2660374077968299</v>
+        <v>0.1874798657372594</v>
       </c>
       <c r="O42" t="n">
-        <v>0.5604648916050792</v>
+        <v>0.6006772108376026</v>
       </c>
       <c r="P42" t="n">
-        <v>0.3862526910379529</v>
+        <v>0.2335616573691368</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.5307759363204241</v>
+        <v>0.575586125254631</v>
       </c>
       <c r="R42" t="n">
-        <v>0.4327807081863284</v>
+        <v>0.3860309943556785</v>
       </c>
       <c r="S42" t="n">
-        <v>0.5570584610104561</v>
+        <v>0.2746726106852293</v>
       </c>
       <c r="T42" t="n">
-        <v>0.7773628681898117</v>
+        <v>0.8233945071697235</v>
       </c>
       <c r="U42" t="n">
-        <v>0.4182024709880352</v>
+        <v>0.5052393767982721</v>
       </c>
       <c r="V42" t="n">
-        <v>0.4947433127090335</v>
+        <v>0.4017011753749102</v>
       </c>
       <c r="W42" t="n">
-        <v>0.5074924528598785</v>
+        <v>0.6329867336899042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>